<commit_message>
Update .gitignore to properly ignore .env file
</commit_message>
<xml_diff>
--- a/stocks_posts_cleaned.xlsx
+++ b/stocks_posts_cleaned.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>102341</v>
+        <v>102350</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>88956</v>
+        <v>88955</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45649</v>
+        <v>45654</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>44006</v>
+        <v>44008</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42057</v>
+        <v>42053</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>36199</v>
+        <v>36194</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27615</v>
+        <v>27616</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26725</v>
+        <v>26724</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26281</v>
+        <v>26280</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25726</v>
+        <v>25729</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>25552</v>
+        <v>25555</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1054,7 +1054,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>22490</v>
+        <v>22486</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>21914</v>
+        <v>21915</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>21854</v>
+        <v>21857</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>21138</v>
+        <v>21135</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>20856</v>
+        <v>20853</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18177</v>
+        <v>18174</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>18082</v>
+        <v>18083</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17108</v>
+        <v>17107</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>16473</v>
+        <v>16471</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>15530</v>
+        <v>15521</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>15218</v>
+        <v>15220</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>15151</v>
+        <v>15149</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>14646</v>
+        <v>14653</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>14367</v>
+        <v>14357</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>13997</v>
+        <v>13996</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>13974</v>
+        <v>13980</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>12800</v>
+        <v>12803</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>12543</v>
+        <v>12550</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1916,7 +1916,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>12489</v>
+        <v>12494</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>12246</v>
+        <v>12240</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11965</v>
+        <v>11968</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>11726</v>
+        <v>11724</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>11485</v>
+        <v>11479</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>10951</v>
+        <v>10956</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>10716</v>
+        <v>10710</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>10655</v>
+        <v>10651</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10542</v>
+        <v>10537</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>10349</v>
+        <v>10351</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>10288</v>
+        <v>10283</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>10176</v>
+        <v>10171</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2469,7 +2469,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10086</v>
+        <v>10090</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2508,7 +2508,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10009</v>
+        <v>10014</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>9915</v>
+        <v>9903</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>9734</v>
+        <v>9741</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2636,7 +2636,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>9725</v>
+        <v>9726</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>9670</v>
+        <v>9664</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2715,7 +2715,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>9639</v>
+        <v>9640</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2755,7 +2755,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>9591</v>
+        <v>9585</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2825,7 +2825,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>9506</v>
+        <v>9510</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>9493</v>
+        <v>9494</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>9410</v>
+        <v>9413</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2944,7 +2944,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>9106</v>
+        <v>9105</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -3028,7 +3028,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>9010</v>
+        <v>9013</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>8969</v>
+        <v>8966</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -3110,7 +3110,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>8756</v>
+        <v>8754</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>8494</v>
+        <v>8493</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -3187,7 +3187,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>8212</v>
+        <v>8211</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -3256,7 +3256,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>8212</v>
+        <v>8209</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -3294,7 +3294,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>8095</v>
+        <v>8099</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3334,7 +3334,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>7997</v>
+        <v>7996</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -3375,7 +3375,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>7912</v>
+        <v>7910</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>7873</v>
+        <v>7867</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>7812</v>
+        <v>7813</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>7808</v>
+        <v>7818</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>7768</v>
+        <v>7765</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>7743</v>
+        <v>7746</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -3706,7 +3706,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7709</v>
+        <v>7703</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -3746,7 +3746,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>7636</v>
+        <v>7632</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -3788,7 +3788,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>7530</v>
+        <v>7523</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3825,7 +3825,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>7467</v>
+        <v>7456</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -4008,7 +4008,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>7447</v>
+        <v>7434</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -4047,7 +4047,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>7427</v>
+        <v>7439</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>7366</v>
+        <v>7368</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -4138,7 +4138,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>7281</v>
+        <v>7285</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>7154</v>
+        <v>7156</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>7098</v>
+        <v>7112</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -4304,7 +4304,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>7079</v>
+        <v>7075</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -4345,7 +4345,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>7064</v>
+        <v>7061</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -4386,7 +4386,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>7048</v>
+        <v>7049</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -4426,7 +4426,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>7036</v>
+        <v>7027</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -4490,7 +4490,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>7029</v>
+        <v>7027</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -4530,7 +4530,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>7018</v>
+        <v>7015</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -4572,7 +4572,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>6978</v>
+        <v>6971</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>6966</v>
+        <v>6963</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -4651,7 +4651,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>6952</v>
+        <v>6956</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -4694,7 +4694,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>6923</v>
+        <v>6929</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -4737,7 +4737,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>6848</v>
+        <v>6851</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -4776,7 +4776,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>6825</v>
+        <v>6833</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -4835,7 +4835,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>6815</v>
+        <v>6817</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -4881,7 +4881,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>6799</v>
+        <v>6794</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>6738</v>
+        <v>6725</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -4986,7 +4986,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6707</v>
+        <v>6705</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>

</xml_diff>